<commit_message>
this is tc of goldclub account creation
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/TestUsers.xlsx
+++ b/src/main/resources/testdata/TestUsers.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A51E314-3982-4677-A4EE-B58FF543D941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,25 +20,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Test@123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>sparrow</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>5th street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>california</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>thomas@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Second@123</t>
+  </si>
+  <si>
+    <t>cpassword</t>
+  </si>
+  <si>
+    <t>marketinginterests</t>
+  </si>
+  <si>
+    <t>Hotels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +110,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,9 +144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -358,24 +428,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -383,10 +457,101 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>90231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{7C42152A-1314-451E-8013-D2CE887E15D0}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{6F4B5638-F7DA-47E2-BC5E-D4FA4F375771}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{9795C857-9FC3-4DE1-8CF0-14C931660387}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>